<commit_message>
amended bowelfunction mapping to improve consistancy extensionmapping
</commit_message>
<xml_diff>
--- a/Mappings/BladderFunction - STU3.xlsx
+++ b/Mappings/BladderFunction - STU3.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="193">
   <si>
     <t>Subject</t>
   </si>
@@ -522,12 +522,6 @@
     <t>.urinaryStoma (extension, reference to ZIB Stoma)</t>
   </si>
   <si>
-    <t>.urineCatheter (extension, reference to MedicalDevice)</t>
-  </si>
-  <si>
-    <t>.incontinenceMaterial (extension, reference to MedicalDevice)</t>
-  </si>
-  <si>
     <t>.comment</t>
   </si>
   <si>
@@ -599,6 +593,22 @@
   </si>
   <si>
     <t>Snapshot of current bladder function. Observation is best fit.</t>
+  </si>
+  <si>
+    <t>.urineCatheter, where:
+• .urineCatheter (extension http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)
+• .urineCatheter.valueReference (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice-UrineCatheter)
+--&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice)</t>
+  </si>
+  <si>
+    <t>.incontinenceMaterial, where
+• .incontinenceMaterial (extension http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.urineCatheter.valueReference.device.type, where
+• .urineCatheter.valueReference.device (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct-UrineCatheter)
+--&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct)
+</t>
   </si>
 </sst>
 </file>
@@ -736,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -793,15 +803,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -956,7 +969,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -997,7 +1010,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1038,7 +1051,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2732,10 +2745,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -2961,95 +2974,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="O1" s="20"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="C2" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="O1" s="21"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D4" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="C8" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="C9" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C10" s="23"/>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
         <v>184</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C10" s="24"/>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3729,8 +3742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3744,8 +3757,9 @@
     <col min="13" max="13" width="75" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="16" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="51.140625" customWidth="1"/>
+    <col min="16" max="16" width="108.140625" customWidth="1"/>
+    <col min="17" max="17" width="96.7109375" customWidth="1"/>
+    <col min="18" max="18" width="51.140625" customWidth="1"/>
     <col min="19" max="19" width="30" customWidth="1"/>
     <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
@@ -3787,13 +3801,13 @@
         <v>163</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>69</v>
@@ -3832,7 +3846,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="T3" s="4"/>
     </row>
@@ -3870,13 +3884,13 @@
         <v>84</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q4" s="19" t="s">
         <v>2</v>
       </c>
       <c r="R4" s="19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="2"/>
@@ -3920,7 +3934,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>92</v>
@@ -3951,15 +3965,15 @@
       <c r="O6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P6" s="16" t="s">
-        <v>166</v>
+      <c r="P6" s="25" t="s">
+        <v>190</v>
       </c>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
       <c r="S6" s="3"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20" ht="51" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -3988,7 +4002,9 @@
       <c r="O7" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="P7" s="16"/>
+      <c r="P7" s="25" t="s">
+        <v>192</v>
+      </c>
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
       <c r="S7" s="3"/>
@@ -4025,8 +4041,8 @@
       <c r="O8" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="16" t="s">
-        <v>167</v>
+      <c r="P8" s="25" t="s">
+        <v>191</v>
       </c>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
@@ -4065,11 +4081,11 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -4105,15 +4121,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
@@ -4262,16 +4278,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
@@ -4412,6 +4428,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4602,12 +4624,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4618,6 +4634,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B314973-BFED-4AE1-8BFD-D3AE1BFE1814}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4636,23 +4669,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEED1E24-4566-4A04-A3A6-B4CDF6B5E3E7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
removed mapping to extension zib-medicaldevice
</commit_message>
<xml_diff>
--- a/Mappings/BladderFunction - STU3.xlsx
+++ b/Mappings/BladderFunction - STU3.xlsx
@@ -16,12 +16,12 @@
     <sheet name="UrineContinenceCodelist" sheetId="6" r:id="rId7"/>
     <sheet name="Terms of Use" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="194">
   <si>
     <t>Subject</t>
   </si>
@@ -595,19 +595,27 @@
     <t>Snapshot of current bladder function. Observation is best fit.</t>
   </si>
   <si>
-    <t>.urineCatheter, where:
-• .urineCatheter (extension http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)
-• .urineCatheter.valueReference (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice-UrineCatheter)
---&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice)</t>
-  </si>
-  <si>
     <t>.incontinenceMaterial, where
 • .incontinenceMaterial (extension http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)</t>
   </si>
   <si>
-    <t xml:space="preserve">.urineCatheter.valueReference.device.type, where
-• .urineCatheter.valueReference.device (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct-UrineCatheter)
+    <t>In zib-medicaldevice it will be possible to refer to this Observation (the reason for using medical product is this observation, where:
+• extension zib-medicalproduct =  http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)
+• .valueReference (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice-UrineCatheter)
+--&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;zib-medicalproduct&gt;.valueReference.device.type, where
+• &lt;zib-medicalproduct&gt;.valueReference.device (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct-UrineCatheter)
 --&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HL7 FHIR R4 relates the resource Observation to DeviceUseStatement as a reason for the usage of this device.
+This relationship is different than in our HCIM's, where the relationship is: Observation is present, and the DeviceUseStatement treats this Observation. 
+i.e.: HCIM = Observation refers to MedicalDeviceStatement
+         FHIR = MedicalDeviceStatement refers to Observation
+FHIR does not allow crossreferences. We decided to go for the FHIR-way and refer to the Observation in MedicalDeviceStatement.
 </t>
   </si>
 </sst>
@@ -969,7 +977,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1010,7 +1018,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1051,7 +1059,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3742,8 +3750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6:P7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3934,7 +3942,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="2:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20" ht="280.5" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>92</v>
@@ -3966,14 +3974,16 @@
         <v>97</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
-      <c r="S6" s="3"/>
+      <c r="S6" s="19" t="s">
+        <v>193</v>
+      </c>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="2:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -4006,8 +4016,6 @@
         <v>192</v>
       </c>
       <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="3"/>
       <c r="T7" s="2"/>
     </row>
     <row r="8" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
@@ -4042,7 +4050,7 @@
         <v>109</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
@@ -4428,6 +4436,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4618,12 +4632,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4634,6 +4642,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B314973-BFED-4AE1-8BFD-D3AE1BFE1814}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4652,23 +4677,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEED1E24-4566-4A04-A3A6-B4CDF6B5E3E7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
amended mapping, removed reference to DeviceUseStatement
</commit_message>
<xml_diff>
--- a/Mappings/BladderFunction - STU3.xlsx
+++ b/Mappings/BladderFunction - STU3.xlsx
@@ -595,28 +595,31 @@
     <t>Snapshot of current bladder function. Observation is best fit.</t>
   </si>
   <si>
-    <t>.incontinenceMaterial, where
-• .incontinenceMaterial (extension http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)</t>
-  </si>
-  <si>
-    <t>In zib-medicaldevice it will be possible to refer to this Observation (the reason for using medical product is this observation, where:
-• extension zib-medicalproduct =  http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)
-• .valueReference (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice-UrineCatheter)
---&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;zib-medicalproduct&gt;.valueReference.device.type, where
-• &lt;zib-medicalproduct&gt;.valueReference.device (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct-UrineCatheter)
---&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">HL7 FHIR R4 relates the resource Observation to DeviceUseStatement as a reason for the usage of this device.
-This relationship is different than in our HCIM's, where the relationship is: Observation is present, and the DeviceUseStatement treats this Observation. 
+This relationship is different than in our HCIM's, where the relationship is: Observation is present, and the DeviceUseStatement is used to counter this Observation. 
 i.e.: HCIM = Observation refers to MedicalDeviceStatement
          FHIR = MedicalDeviceStatement refers to Observation
 FHIR does not allow crossreferences. We decided to go for the FHIR-way and refer to the Observation in MedicalDeviceStatement.
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No reference in this profile., but in the profile zib-medicalproduct (DeviceUseStatement) 
+&lt;zib-medicalproduct&gt;.valueReference.device.type, where
+• &lt;zib-medicalproduct&gt;.valueReference.device (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct-UrineCatheter)
+--&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct)
+</t>
+  </si>
+  <si>
+    <t>No reference in this profile., but in the profile zib-medicalproduct (DeviceUseStatement) 
+In zib-medicaldevice it will be possible to refer to this Observation (the reason for using medical product is this observation, where:
+• extension zib-medicalproduct =  http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)
+• .valueReference (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice-UrineCatheter)
+--&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice)</t>
+  </si>
+  <si>
+    <t>No reference in this profile., but in the profile zib-medicalproduct (DeviceUseStatement) 
+In zib-medicaldevice it will be possible to refer to this Observation (the reason for using medical product is this observation, where:
+• extension zib-medicalproduct =  http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)</t>
   </si>
 </sst>
 </file>
@@ -977,7 +980,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1018,7 +1021,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1059,7 +1062,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3750,8 +3753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3768,7 +3771,7 @@
     <col min="16" max="16" width="108.140625" customWidth="1"/>
     <col min="17" max="17" width="96.7109375" customWidth="1"/>
     <col min="18" max="18" width="51.140625" customWidth="1"/>
-    <col min="19" max="19" width="30" customWidth="1"/>
+    <col min="19" max="19" width="59.85546875" customWidth="1"/>
     <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3942,7 +3945,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="2:20" ht="280.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>92</v>
@@ -3974,16 +3977,16 @@
         <v>97</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
       <c r="S6" s="19" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="2:20" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -4013,12 +4016,12 @@
         <v>103</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q7" s="16"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:20" ht="51" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
         <v>104</v>
@@ -4050,7 +4053,7 @@
         <v>109</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
@@ -4436,12 +4439,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4632,6 +4629,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4642,23 +4645,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B314973-BFED-4AE1-8BFD-D3AE1BFE1814}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4677,6 +4663,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEED1E24-4566-4A04-A3A6-B4CDF6B5E3E7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fix: typo in excel
</commit_message>
<xml_diff>
--- a/Mappings/BladderFunction - STU3.xlsx
+++ b/Mappings/BladderFunction - STU3.xlsx
@@ -519,9 +519,6 @@
 (.code = definitionCode)</t>
   </si>
   <si>
-    <t>.urinaryStoma (extension, reference to ZIB Stoma)</t>
-  </si>
-  <si>
     <t>.comment</t>
   </si>
   <si>
@@ -620,6 +617,10 @@
     <t>No reference in this profile., but in the profile zib-medicalproduct (DeviceUseStatement) 
 In zib-medicaldevice it will be possible to refer to this Observation (the reason for using medical product is this observation, where:
 • extension zib-medicalproduct =  http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)</t>
+  </si>
+  <si>
+    <t>.urinaryStoma (extension, reference to ZIB Stoma)
+• extension zib-BladderFunction-Stoma =  http://nictiz.nl/fhir/StructureDefinition/zib-BladderFunction-Stoma)</t>
   </si>
 </sst>
 </file>
@@ -980,7 +981,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1021,7 +1022,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1062,7 +1063,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2986,19 +2987,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
@@ -3007,64 +3008,64 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>175</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>182</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -3073,7 +3074,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3753,8 +3754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3812,13 +3813,13 @@
         <v>163</v>
       </c>
       <c r="Q2" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="R2" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="R2" s="18" t="s">
-        <v>187</v>
-      </c>
       <c r="S2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>69</v>
@@ -3857,7 +3858,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T3" s="4"/>
     </row>
@@ -3895,13 +3896,13 @@
         <v>84</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q4" s="19" t="s">
         <v>2</v>
       </c>
       <c r="R4" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="2"/>
@@ -3938,7 +3939,7 @@
         <v>91</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="Q5" s="17"/>
       <c r="R5" s="17"/>
@@ -3977,12 +3978,12 @@
         <v>97</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
       <c r="S6" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T6" s="2"/>
     </row>
@@ -4016,7 +4017,7 @@
         <v>103</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q7" s="16"/>
       <c r="T7" s="2"/>
@@ -4053,7 +4054,7 @@
         <v>109</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
@@ -4092,11 +4093,11 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -4439,6 +4440,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4629,12 +4636,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4645,6 +4646,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B314973-BFED-4AE1-8BFD-D3AE1BFE1814}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4663,23 +4681,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEED1E24-4566-4A04-A3A6-B4CDF6B5E3E7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fix: changed location of reference to zib-Stoma to .related.target
</commit_message>
<xml_diff>
--- a/Mappings/BladderFunction - STU3.xlsx
+++ b/Mappings/BladderFunction - STU3.xlsx
@@ -619,8 +619,7 @@
 • extension zib-medicalproduct =  http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)</t>
   </si>
   <si>
-    <t>.urinaryStoma (extension, reference to ZIB Stoma)
-• extension zib-BladderFunction-Stoma =  http://nictiz.nl/fhir/StructureDefinition/zib-BladderFunction-Stoma)</t>
+    <t>.related.target</t>
   </si>
 </sst>
 </file>
@@ -981,7 +980,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1022,7 +1021,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1063,7 +1062,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3754,8 +3753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4440,12 +4439,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4636,6 +4629,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4646,23 +4645,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B314973-BFED-4AE1-8BFD-D3AE1BFE1814}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4681,6 +4663,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A50E9710-B5BD-42E5-85A7-6C3412C38BE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEED1E24-4566-4A04-A3A6-B4CDF6B5E3E7}">
   <ds:schemaRefs>

</xml_diff>